<commit_message>
Add Validaciones vehiculoExcel y permisos según el rol
</commit_message>
<xml_diff>
--- a/files/excel prueba.xlsx
+++ b/files/excel prueba.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="45">
   <si>
     <t>placa</t>
   </si>
@@ -59,57 +59,122 @@
     <t>22DFD</t>
   </si>
   <si>
+    <t>Rojo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Daño carrocería </t>
+  </si>
+  <si>
+    <t>ACTIVO</t>
+  </si>
+  <si>
+    <t>49NJD</t>
+  </si>
+  <si>
+    <t>Amarillo</t>
+  </si>
+  <si>
+    <t>Daño puerta</t>
+  </si>
+  <si>
+    <t>89KJD</t>
+  </si>
+  <si>
+    <t>Mitsubishi</t>
+  </si>
+  <si>
+    <t>Detalles varios</t>
+  </si>
+  <si>
+    <t>Azul.png</t>
+  </si>
+  <si>
+    <t>Amarillo.png</t>
+  </si>
+  <si>
+    <t>Verde</t>
+  </si>
+  <si>
+    <t>Verde.png</t>
+  </si>
+  <si>
+    <t>54MNF</t>
+  </si>
+  <si>
+    <t>Daño en la puerta</t>
+  </si>
+  <si>
+    <t>Amrillo.png</t>
+  </si>
+  <si>
+    <t>Suzuki</t>
+  </si>
+  <si>
+    <t>Toyota</t>
+  </si>
+  <si>
+    <t>90ASD</t>
+  </si>
+  <si>
+    <t>Full</t>
+  </si>
+  <si>
+    <t>Daño en el tanque</t>
+  </si>
+  <si>
+    <t>49NJDY</t>
+  </si>
+  <si>
+    <t>Corolla</t>
+  </si>
+  <si>
+    <t>Azul</t>
+  </si>
+  <si>
+    <t>Daños varios</t>
+  </si>
+  <si>
     <t>Mazda</t>
   </si>
   <si>
-    <t>Rojo</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Daño carrocería </t>
-  </si>
-  <si>
-    <t>azul.png</t>
-  </si>
-  <si>
-    <t>ACTIVO</t>
-  </si>
-  <si>
-    <t>49NJD</t>
-  </si>
-  <si>
-    <t>Chevrolet</t>
-  </si>
-  <si>
-    <t>Amarillo</t>
-  </si>
-  <si>
-    <t>Daño puerta</t>
-  </si>
-  <si>
-    <t>amarillo.png</t>
-  </si>
-  <si>
-    <t>89KJD</t>
-  </si>
-  <si>
-    <t>Mitsubishi</t>
-  </si>
-  <si>
-    <t>Jasmin</t>
-  </si>
-  <si>
-    <t>Detalles varios</t>
-  </si>
-  <si>
-    <t>jasmin.png</t>
+    <t>MJHD18</t>
+  </si>
+  <si>
+    <t>Muras</t>
+  </si>
+  <si>
+    <t>Manila</t>
+  </si>
+  <si>
+    <t>Rojo.png</t>
+  </si>
+  <si>
+    <t>OIOJAJS</t>
+  </si>
+  <si>
+    <t>Lambo</t>
+  </si>
+  <si>
+    <t>Vidrio</t>
+  </si>
+  <si>
+    <t>asd</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -137,9 +202,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -420,21 +488,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J4"/>
+  <dimension ref="A1:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="15" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="12.140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="13.5703125" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="17.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -466,27 +534,27 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>10</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="C2">
         <v>1999</v>
       </c>
       <c r="D2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E2" t="s">
         <v>12</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
+        <v>20</v>
+      </c>
+      <c r="G2" t="s">
         <v>13</v>
-      </c>
-      <c r="F2" t="s">
-        <v>14</v>
-      </c>
-      <c r="G2" t="s">
-        <v>15</v>
       </c>
       <c r="H2">
         <v>200000</v>
@@ -498,27 +566,27 @@
         <v>44420</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>17</v>
+        <v>36</v>
       </c>
       <c r="C3">
         <v>1997</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="E3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="F3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="G3" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H3">
         <v>240000</v>
@@ -530,27 +598,27 @@
         <v>44420</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="B4" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C4">
         <v>2000</v>
       </c>
       <c r="D4" t="s">
+        <v>22</v>
+      </c>
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4" t="s">
         <v>23</v>
       </c>
-      <c r="E4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F4" t="s">
-        <v>25</v>
-      </c>
       <c r="G4" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="H4">
         <v>210000</v>
@@ -560,6 +628,167 @@
       </c>
       <c r="J4" s="1">
         <v>44421</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B5" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5">
+        <v>1985</v>
+      </c>
+      <c r="D5" t="s">
+        <v>15</v>
+      </c>
+      <c r="E5" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5">
+        <v>200</v>
+      </c>
+      <c r="I5" s="1">
+        <v>44422</v>
+      </c>
+      <c r="J5" s="1">
+        <v>44422</v>
+      </c>
+      <c r="L5" s="2"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>29</v>
+      </c>
+      <c r="B6" t="s">
+        <v>30</v>
+      </c>
+      <c r="C6">
+        <v>1997</v>
+      </c>
+      <c r="D6" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" t="s">
+        <v>23</v>
+      </c>
+      <c r="G6" t="s">
+        <v>13</v>
+      </c>
+      <c r="H6">
+        <v>236</v>
+      </c>
+      <c r="I6" s="3">
+        <v>44423</v>
+      </c>
+      <c r="J6" s="1">
+        <v>44423</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>32</v>
+      </c>
+      <c r="B7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C7">
+        <v>1997</v>
+      </c>
+      <c r="D7" t="s">
+        <v>34</v>
+      </c>
+      <c r="E7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" t="s">
+        <v>20</v>
+      </c>
+      <c r="G7" t="s">
+        <v>13</v>
+      </c>
+      <c r="H7">
+        <v>58</v>
+      </c>
+      <c r="I7" s="1">
+        <v>44423</v>
+      </c>
+      <c r="J7" s="1">
+        <v>44423</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>37</v>
+      </c>
+      <c r="B8" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8">
+        <v>1996</v>
+      </c>
+      <c r="D8" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" t="s">
+        <v>40</v>
+      </c>
+      <c r="G8" t="s">
+        <v>13</v>
+      </c>
+      <c r="H8">
+        <v>784</v>
+      </c>
+      <c r="I8" s="1">
+        <v>44424</v>
+      </c>
+      <c r="J8" s="1">
+        <v>44424</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C9">
+        <v>2000</v>
+      </c>
+      <c r="D9" t="s">
+        <v>15</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="F9" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="G9" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="H9" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="I9" s="1">
+        <v>44424</v>
+      </c>
+      <c r="J9" s="1">
+        <v>44424</v>
       </c>
     </row>
   </sheetData>

</xml_diff>